<commit_message>
excel template / linear model automation
</commit_message>
<xml_diff>
--- a/input_couches.xlsx
+++ b/input_couches.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JUSAU\Desktop\LANG_SCRIPT\LangageScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FEB716-998A-4B6C-B4F9-B6D1552C9712}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02CF0C2-6D69-4EB8-B7DB-A8607F8E6ACA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6000" yWindow="1815" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
   <si>
     <t>a- Joone</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>Score</t>
+  </si>
+  <si>
+    <t>Coefficient</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Min_value</t>
+  </si>
+  <si>
+    <t>Max_value</t>
   </si>
 </sst>
 </file>
@@ -453,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -465,9 +477,12 @@
     <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.625" customWidth="1"/>
+    <col min="5" max="5" width="15.25" customWidth="1"/>
+    <col min="6" max="6" width="14.75" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -480,8 +495,20 @@
       <c r="D1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,8 +521,20 @@
       <c r="D2" s="3">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>0.6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>17</v>
+      </c>
+      <c r="H2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -508,8 +547,20 @@
       <c r="D3" s="3">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>0.4</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3">
+        <v>13</v>
+      </c>
+      <c r="H3">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -522,8 +573,17 @@
       <c r="D4" s="3">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -536,8 +596,17 @@
       <c r="D5" s="3">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5">
+        <v>7</v>
+      </c>
+      <c r="H5">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -550,8 +619,17 @@
       <c r="D6" s="3">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -565,7 +643,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -579,7 +657,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -593,7 +671,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -607,7 +685,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -621,7 +699,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -635,7 +713,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>